<commit_message>
MIMS analysis and TS Ophelia analysis.
</commit_message>
<xml_diff>
--- a/data/MIMS/Oct24/CalculatedWaterColumn_outputs.xlsx
+++ b/data/MIMS/Oct24/CalculatedWaterColumn_outputs.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinfinlay/GitHub/TownCreekWater/data/MIMS/Oct24/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC296ABA-F3AC-F44B-809F-A6A2D4CF2445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B2B149-4C1E-A94A-8F07-C7C3269E0103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="3700" windowWidth="26840" windowHeight="15940" xr2:uid="{81EF9C1B-2FC8-D84F-8E4D-1EE53E8D724D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{81EF9C1B-2FC8-D84F-8E4D-1EE53E8D724D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>uM N</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>Index</t>
+  </si>
+  <si>
+    <t>NetNratio</t>
   </si>
 </sst>
 </file>
@@ -507,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB6497DA-186C-8340-B7CC-34A0C10517FD}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -519,9 +522,10 @@
     <col min="2" max="3" width="21" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -561,8 +565,11 @@
       <c r="M1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -604,8 +611,12 @@
       <c r="M2">
         <v>7.2555613390027522</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2">
+        <f>D2/I2</f>
+        <v>0.99602051896937449</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -647,8 +658,12 @@
       <c r="M3">
         <v>7.3783487867446258</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3">
+        <f t="shared" ref="N3:N19" si="2">D3/I3</f>
+        <v>1.0011886287399272</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -690,8 +705,12 @@
       <c r="M4">
         <v>7.4278699420001102</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4">
+        <f t="shared" si="2"/>
+        <v>0.99200194847779077</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -733,8 +752,12 @@
       <c r="M5">
         <v>6.880436534942028</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5">
+        <f t="shared" si="2"/>
+        <v>1.0031859641271008</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -776,8 +799,12 @@
       <c r="M6">
         <v>6.803203308650529</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N6">
+        <f t="shared" si="2"/>
+        <v>1.0003586763656993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -819,8 +846,12 @@
       <c r="M7">
         <v>7.9608630487895411</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N7">
+        <f t="shared" si="2"/>
+        <v>0.99879177230196081</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -862,8 +893,12 @@
       <c r="M8">
         <v>7.4093461268021104</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N8">
+        <f t="shared" si="2"/>
+        <v>0.99749343243949307</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -905,8 +940,12 @@
       <c r="M9">
         <v>7.2145505585889724</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N9">
+        <f t="shared" si="2"/>
+        <v>0.99556925311878963</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -948,8 +987,12 @@
       <c r="M10">
         <v>7.3951841152331674</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N10">
+        <f t="shared" si="2"/>
+        <v>1.0003129913646434</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -991,8 +1034,12 @@
       <c r="M11">
         <v>8.2711688065969149</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N11">
+        <f t="shared" si="2"/>
+        <v>1.008800907748582</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1034,8 +1081,12 @@
       <c r="M12">
         <v>7.9375737446140811</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N12">
+        <f t="shared" si="2"/>
+        <v>1.0062655669764851</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1077,8 +1128,12 @@
       <c r="M13">
         <v>7.9610053956531956</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N13">
+        <f t="shared" si="2"/>
+        <v>1.0044003912536463</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -1120,8 +1175,12 @@
       <c r="M14">
         <v>8.036259595288497</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N14">
+        <f t="shared" si="2"/>
+        <v>1.0046740578714357</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1163,8 +1222,12 @@
       <c r="M15">
         <v>8.1859283293035841</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N15">
+        <f t="shared" si="2"/>
+        <v>1.002305387377322</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -1206,8 +1269,12 @@
       <c r="M16">
         <v>8.3454078198533495</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N16">
+        <f t="shared" si="2"/>
+        <v>1.0018680826066673</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1249,8 +1316,12 @@
       <c r="M17">
         <v>8.1035428811154535</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N17">
+        <f t="shared" si="2"/>
+        <v>1.0033264675365361</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1292,8 +1363,12 @@
       <c r="M18">
         <v>7.7063150295692351</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N18">
+        <f t="shared" si="2"/>
+        <v>0.98188899219876347</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -1334,6 +1409,10 @@
       </c>
       <c r="M19">
         <v>7.7676371567466997</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="2"/>
+        <v>0.97615754875638472</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
N saturation ratios figure and calculations.
</commit_message>
<xml_diff>
--- a/data/MIMS/Oct24/CalculatedWaterColumn_outputs.xlsx
+++ b/data/MIMS/Oct24/CalculatedWaterColumn_outputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinfinlay/GitHub/TownCreekWater/data/MIMS/Oct24/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B2B149-4C1E-A94A-8F07-C7C3269E0103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6263A59A-95E2-534D-8713-514A14510F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{81EF9C1B-2FC8-D84F-8E4D-1EE53E8D724D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20460" xr2:uid="{81EF9C1B-2FC8-D84F-8E4D-1EE53E8D724D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>uM N</t>
   </si>
@@ -131,7 +131,16 @@
     <t>Index</t>
   </si>
   <si>
-    <t>NetNratio</t>
+    <t>Net_N2Ar_ratio</t>
+  </si>
+  <si>
+    <t>uM N2</t>
+  </si>
+  <si>
+    <t>uM N2 field expected</t>
+  </si>
+  <si>
+    <t>NsatRatio</t>
   </si>
 </sst>
 </file>
@@ -510,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB6497DA-186C-8340-B7CC-34A0C10517FD}">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -522,10 +531,11 @@
     <col min="2" max="3" width="21" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -568,8 +578,17 @@
       <c r="N1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -615,8 +634,18 @@
         <f>D2/I2</f>
         <v>0.99602051896937449</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O2">
+        <v>505.06908116308688</v>
+      </c>
+      <c r="P2">
+        <v>507.08702435739349</v>
+      </c>
+      <c r="Q2">
+        <f>O2/P2</f>
+        <v>0.99602051896937449</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -662,8 +691,18 @@
         <f t="shared" ref="N3:N19" si="2">D3/I3</f>
         <v>1.0011886287399272</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O3">
+        <v>507.68976256818883</v>
+      </c>
+      <c r="P3">
+        <v>507.08702435739349</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q19" si="3">O3/P3</f>
+        <v>1.0011886287399272</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -709,8 +748,18 @@
         <f t="shared" si="2"/>
         <v>0.99200194847779077</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O4">
+        <v>503.03131621033924</v>
+      </c>
+      <c r="P4">
+        <v>507.08702435739349</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="3"/>
+        <v>0.99200194847779066</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -756,8 +805,18 @@
         <f t="shared" si="2"/>
         <v>1.0031859641271008</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O5">
+        <v>508.70258542631433</v>
+      </c>
+      <c r="P5">
+        <v>507.08702435739349</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="3"/>
+        <v>1.0031859641271006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -803,8 +862,18 @@
         <f t="shared" si="2"/>
         <v>1.0003586763656993</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O6">
+        <v>507.26890448838327</v>
+      </c>
+      <c r="P6">
+        <v>507.08702435739349</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="3"/>
+        <v>1.0003586763656993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -850,8 +919,18 @@
         <f t="shared" si="2"/>
         <v>0.99879177230196081</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O7">
+        <v>506.4743477692486</v>
+      </c>
+      <c r="P7">
+        <v>507.08702435739349</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="3"/>
+        <v>0.99879177230196081</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -897,8 +976,18 @@
         <f t="shared" si="2"/>
         <v>0.99749343243949307</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O8">
+        <v>505.81597647178523</v>
+      </c>
+      <c r="P8">
+        <v>507.08702435739349</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="3"/>
+        <v>0.99749343243949307</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -944,8 +1033,18 @@
         <f t="shared" si="2"/>
         <v>0.99556925311878963</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O9">
+        <v>504.84025010571969</v>
+      </c>
+      <c r="P9">
+        <v>507.08702435739349</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="3"/>
+        <v>0.99556925311878952</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -991,8 +1090,18 @@
         <f t="shared" si="2"/>
         <v>1.0003129913646434</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O10">
+        <v>507.24573821714</v>
+      </c>
+      <c r="P10">
+        <v>507.08702435739349</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="3"/>
+        <v>1.0003129913646434</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1038,8 +1147,18 @@
         <f t="shared" si="2"/>
         <v>1.008800907748582</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O11">
+        <v>511.54985047926579</v>
+      </c>
+      <c r="P11">
+        <v>507.08702435739349</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="3"/>
+        <v>1.0088009077485818</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -1085,8 +1204,18 @@
         <f t="shared" si="2"/>
         <v>1.0062655669764851</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O12">
+        <v>510.26421207141124</v>
+      </c>
+      <c r="P12">
+        <v>507.08702435739349</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="3"/>
+        <v>1.0062655669764851</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1132,8 +1261,18 @@
         <f t="shared" si="2"/>
         <v>1.0044003912536463</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O13">
+        <v>509.31840566421323</v>
+      </c>
+      <c r="P13">
+        <v>507.08702435739349</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="3"/>
+        <v>1.0044003912536461</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
@@ -1179,8 +1318,18 @@
         <f t="shared" si="2"/>
         <v>1.0046740578714357</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O14">
+        <v>509.45717845509409</v>
+      </c>
+      <c r="P14">
+        <v>507.08702435739349</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="3"/>
+        <v>1.0046740578714357</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -1226,8 +1375,18 @@
         <f t="shared" si="2"/>
         <v>1.002305387377322</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O15">
+        <v>508.25605638255075</v>
+      </c>
+      <c r="P15">
+        <v>507.08702435739349</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="3"/>
+        <v>1.002305387377322</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -1273,8 +1432,18 @@
         <f t="shared" si="2"/>
         <v>1.0018680826066673</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O16">
+        <v>508.03430480766212</v>
+      </c>
+      <c r="P16">
+        <v>507.08702435739349</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="3"/>
+        <v>1.001868082606667</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1320,8 +1489,18 @@
         <f t="shared" si="2"/>
         <v>1.0033264675365361</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O17">
+        <v>508.77383288211701</v>
+      </c>
+      <c r="P17">
+        <v>507.08702435739349</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="3"/>
+        <v>1.0033264675365361</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
@@ -1367,8 +1546,18 @@
         <f t="shared" si="2"/>
         <v>0.98188899219876347</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O18">
+        <v>497.90316730335087</v>
+      </c>
+      <c r="P18">
+        <v>507.08702435739349</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="3"/>
+        <v>0.98188899219876336</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -1413,6 +1602,16 @@
       <c r="N19">
         <f t="shared" si="2"/>
         <v>0.97615754875638472</v>
+      </c>
+      <c r="O19">
+        <v>494.99682670288234</v>
+      </c>
+      <c r="P19">
+        <v>507.08702435739349</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="3"/>
+        <v>0.97615754875638461</v>
       </c>
     </row>
   </sheetData>

</xml_diff>